<commit_message>
compare haplotypes with filtered ED50s
</commit_message>
<xml_diff>
--- a/data/collection_metadata.xlsx
+++ b/data/collection_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/TPCBASS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrcunning/Projects/TPCBASS/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFAC4BD-D615-7149-934A-1AA42FEA254B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A83B39-C389-904C-8400-AD2AE8492762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{DA8E9BB7-9B8D-C442-8290-0F73275806AC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="37">
   <si>
     <t>Site</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>W149° 48.380'</t>
+  </si>
+  <si>
+    <t>mtORF</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>TPC2</t>
   </si>
 </sst>
 </file>
@@ -190,7 +202,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -478,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -486,22 +498,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE659553-DE02-6F4F-9368-5A8BEC9EB046}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="14.6640625" customWidth="1"/>
-    <col min="20" max="20" width="25.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="21" max="21" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -527,19 +539,25 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>20221208</v>
       </c>
@@ -564,20 +582,20 @@
       <c r="H2">
         <v>38</v>
       </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20221208</v>
       </c>
@@ -602,21 +620,21 @@
       <c r="H3">
         <v>39</v>
       </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="2"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>20221208</v>
       </c>
@@ -641,20 +659,20 @@
       <c r="H4">
         <v>40</v>
       </c>
-      <c r="I4" t="s">
-        <v>11</v>
-      </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>20221208</v>
       </c>
@@ -679,20 +697,20 @@
       <c r="H5">
         <v>6</v>
       </c>
-      <c r="I5" t="s">
-        <v>11</v>
-      </c>
       <c r="J5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
         <v>27</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20221208</v>
       </c>
@@ -717,20 +735,20 @@
       <c r="H6">
         <v>23</v>
       </c>
-      <c r="I6" t="s">
-        <v>11</v>
-      </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" t="s">
         <v>30</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>20221208</v>
       </c>
@@ -755,21 +773,21 @@
       <c r="H7">
         <v>24</v>
       </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
       <c r="J7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" t="s">
         <v>31</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>32</v>
       </c>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>20221208</v>
       </c>
@@ -794,20 +812,20 @@
       <c r="H8">
         <v>3</v>
       </c>
-      <c r="I8" t="s">
-        <v>11</v>
-      </c>
       <c r="J8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K8" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" t="s">
         <v>31</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>20221208</v>
       </c>
@@ -830,13 +848,19 @@
         <v>32</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20221208</v>
       </c>
@@ -859,13 +883,19 @@
         <v>31</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>20221208</v>
       </c>
@@ -888,13 +918,19 @@
         <v>22</v>
       </c>
       <c r="I11" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>20221208</v>
       </c>
@@ -917,13 +953,19 @@
         <v>29</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="J12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>20221207</v>
       </c>
@@ -946,13 +988,19 @@
         <v>11</v>
       </c>
       <c r="I13" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>20221207</v>
       </c>
@@ -974,14 +1022,14 @@
       <c r="H14">
         <v>17</v>
       </c>
-      <c r="I14" t="s">
-        <v>11</v>
-      </c>
       <c r="J14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>20221207</v>
       </c>
@@ -1004,13 +1052,19 @@
         <v>16</v>
       </c>
       <c r="I15" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>20221207</v>
       </c>
@@ -1033,13 +1087,19 @@
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>20221207</v>
       </c>
@@ -1062,13 +1122,19 @@
         <v>20</v>
       </c>
       <c r="I17" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" t="s">
+        <v>11</v>
+      </c>
+      <c r="N17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>20221207</v>
       </c>
@@ -1091,13 +1157,19 @@
         <v>18</v>
       </c>
       <c r="I18" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>20221207</v>
       </c>
@@ -1120,13 +1192,16 @@
         <v>14</v>
       </c>
       <c r="I19" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20221207</v>
       </c>
@@ -1149,13 +1224,19 @@
         <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K20" t="s">
+        <v>12</v>
+      </c>
+      <c r="N20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20221207</v>
       </c>
@@ -1178,13 +1259,19 @@
         <v>13</v>
       </c>
       <c r="I21" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>12</v>
+      </c>
+      <c r="N21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20221207</v>
       </c>
@@ -1207,13 +1294,19 @@
         <v>19</v>
       </c>
       <c r="I22" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
+        <v>12</v>
+      </c>
+      <c r="N22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20221207</v>
       </c>
@@ -1236,13 +1329,19 @@
         <v>37</v>
       </c>
       <c r="I23" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J23" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K23" t="s">
+        <v>12</v>
+      </c>
+      <c r="N23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20221207</v>
       </c>
@@ -1265,13 +1364,19 @@
         <v>34</v>
       </c>
       <c r="I24" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K24" t="s">
+        <v>12</v>
+      </c>
+      <c r="N24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20221207</v>
       </c>
@@ -1294,13 +1399,19 @@
         <v>35</v>
       </c>
       <c r="I25" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="J25" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K25" t="s">
+        <v>12</v>
+      </c>
+      <c r="N25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20221207</v>
       </c>
@@ -1323,13 +1434,16 @@
         <v>36</v>
       </c>
       <c r="I26" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J26" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="K26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20221207</v>
       </c>
@@ -1352,9 +1466,12 @@
         <v>33</v>
       </c>
       <c r="I27" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="J27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>